<commit_message>
Finessing eHBV side data
</commit_message>
<xml_diff>
--- a/tabular/ehbv-refseqs-side-data.xlsx
+++ b/tabular/ehbv-refseqs-side-data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$6</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -45,15 +45,9 @@
     <t>eSNHBV1-con</t>
   </si>
   <si>
-    <t>eCRHBV2</t>
-  </si>
-  <si>
     <t>eCRHBV2-con</t>
   </si>
   <si>
-    <t>Endogenous crocodile hepatitis B virus 2</t>
-  </si>
-  <si>
     <t>Crocodylus</t>
   </si>
   <si>
@@ -66,12 +60,6 @@
     <t>Chrysemys</t>
   </si>
   <si>
-    <t>crocodiles</t>
-  </si>
-  <si>
-    <t>eCRHBV</t>
-  </si>
-  <si>
     <t>eCRHBV-con</t>
   </si>
   <si>
@@ -87,9 +75,6 @@
     <t>Endogenous comodo dragon hepatitis B virus</t>
   </si>
   <si>
-    <t>eTHBV</t>
-  </si>
-  <si>
     <t>eTHBV-con</t>
   </si>
   <si>
@@ -114,9 +99,6 @@
     <t>Varanus komodoensis</t>
   </si>
   <si>
-    <t>eAVHBV1</t>
-  </si>
-  <si>
     <t>eAVHBV1-con</t>
   </si>
   <si>
@@ -132,15 +114,6 @@
     <t>birds</t>
   </si>
   <si>
-    <t>eSpHBV</t>
-  </si>
-  <si>
-    <t>eSphHBV_con</t>
-  </si>
-  <si>
-    <t>sequenceID</t>
-  </si>
-  <si>
     <t>virus_name</t>
   </si>
   <si>
@@ -151,6 +124,12 @@
   </si>
   <si>
     <t>clade</t>
+  </si>
+  <si>
+    <t>SphHBV-con</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -257,8 +236,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="399">
+  <cellStyleXfs count="413">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,7 +661,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="399">
+  <cellStyles count="413">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -868,6 +861,13 @@
     <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1067,6 +1067,13 @@
     <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1404,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G7" sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1423,19 +1430,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -1467,132 +1474,111 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="D7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="7"/>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G10"/>
+  <autoFilter ref="A1:G9"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>